<commit_message>
fix couple of variable names to match the table in overall_plaus
</commit_message>
<xml_diff>
--- a/inst/mort_quality_report/resources/overall_plaus.xlsx
+++ b/inst/mort_quality_report/resources/overall_plaus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\IPHRA_toolkit\cleaning\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\mort_quality_report\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3389AC9-259C-4F81-A323-304AA9D4B40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9BC11A-DF41-4C57-87C6-EABBED625D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FSL" sheetId="1" r:id="rId1"/>
@@ -349,13 +349,13 @@
     <t>plaus_hh_multiple_death</t>
   </si>
   <si>
-    <t>plaus_overall_cdr</t>
-  </si>
-  <si>
     <t>20 &lt; 30</t>
   </si>
   <si>
     <t>&gt;= 30</t>
+  </si>
+  <si>
+    <t>plaus_cdr</t>
   </si>
 </sst>
 </file>
@@ -816,128 +816,128 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1233,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D57" sqref="D57:E57"/>
     </sheetView>
   </sheetViews>
@@ -1246,662 +1246,662 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46"/>
+      <c r="C1" s="62"/>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="46"/>
+      <c r="G1" s="62"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="22" t="s">
+      <c r="B2" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="23"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="48" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="48"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="35">
-        <v>0</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="35">
+      <c r="A3" s="30"/>
+      <c r="B3" s="49">
+        <v>0</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="49">
         <v>4</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="49">
+      <c r="E3" s="50"/>
+      <c r="F3" s="43">
         <v>6</v>
       </c>
-      <c r="G3" s="49"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="31" t="s">
+      <c r="C4" s="59"/>
+      <c r="D4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="26" t="s">
+      <c r="E4" s="59"/>
+      <c r="F4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="35">
-        <v>0</v>
-      </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37">
+      <c r="A6" s="42"/>
+      <c r="B6" s="49">
+        <v>0</v>
+      </c>
+      <c r="C6" s="50"/>
+      <c r="D6" s="41">
         <v>2</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37">
+      <c r="E6" s="41"/>
+      <c r="F6" s="41">
         <v>4</v>
       </c>
-      <c r="G6" s="37"/>
+      <c r="G6" s="41"/>
     </row>
     <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="22" t="s">
+      <c r="B7" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="26" t="s">
+      <c r="E7" s="27"/>
+      <c r="F7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="42">
-        <v>0</v>
-      </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="42">
+      <c r="A8" s="30"/>
+      <c r="B8" s="24">
+        <v>0</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="24">
         <v>2</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="37">
+      <c r="E8" s="25"/>
+      <c r="F8" s="41">
         <v>4</v>
       </c>
-      <c r="G8" s="37"/>
+      <c r="G8" s="41"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="22" t="s">
+      <c r="B9" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="41" t="s">
+      <c r="E9" s="27"/>
+      <c r="F9" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="41"/>
+      <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="42">
-        <v>0</v>
-      </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="42">
+      <c r="A10" s="30"/>
+      <c r="B10" s="24">
+        <v>0</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="24">
         <v>1</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="37">
+      <c r="E10" s="25"/>
+      <c r="F10" s="41">
         <v>2</v>
       </c>
-      <c r="G10" s="37"/>
+      <c r="G10" s="41"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="22" t="s">
+      <c r="B11" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="41" t="s">
+      <c r="E11" s="27"/>
+      <c r="F11" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="41"/>
+      <c r="G11" s="40"/>
     </row>
     <row r="12" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="44"/>
-      <c r="B12" s="27">
-        <v>0</v>
-      </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="27">
+      <c r="A12" s="55"/>
+      <c r="B12" s="28">
+        <v>0</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="28">
         <v>2</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="45">
+      <c r="E12" s="29"/>
+      <c r="F12" s="36">
         <v>4</v>
       </c>
-      <c r="G12" s="45"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="22" t="s">
+      <c r="B13" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="23"/>
+      <c r="D13" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="41" t="s">
+      <c r="E13" s="27"/>
+      <c r="F13" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="41"/>
+      <c r="G13" s="40"/>
     </row>
     <row r="14" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="44"/>
-      <c r="B14" s="27">
-        <v>0</v>
-      </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="27">
+      <c r="A14" s="55"/>
+      <c r="B14" s="28">
+        <v>0</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="28">
         <v>2</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="45">
+      <c r="E14" s="29"/>
+      <c r="F14" s="36">
         <v>4</v>
       </c>
-      <c r="G14" s="45"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="22" t="s">
+      <c r="B15" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="53"/>
+      <c r="D15" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="52" t="s">
+      <c r="E15" s="27"/>
+      <c r="F15" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="52"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="42">
-        <v>0</v>
-      </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="42">
+      <c r="A16" s="30"/>
+      <c r="B16" s="24">
+        <v>0</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="24">
         <v>4</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="37">
+      <c r="E16" s="25"/>
+      <c r="F16" s="41">
         <v>6</v>
       </c>
-      <c r="G16" s="37"/>
+      <c r="G16" s="41"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="31" t="s">
+      <c r="C17" s="59"/>
+      <c r="D17" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="26" t="s">
+      <c r="E17" s="59"/>
+      <c r="F17" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="26"/>
+      <c r="G17" s="32"/>
     </row>
     <row r="18" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="42">
-        <v>0</v>
-      </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="37">
+      <c r="A19" s="42"/>
+      <c r="B19" s="24">
+        <v>0</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="41">
         <v>2</v>
       </c>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37">
+      <c r="E19" s="41"/>
+      <c r="F19" s="41">
         <v>3</v>
       </c>
-      <c r="G19" s="37"/>
+      <c r="G19" s="41"/>
     </row>
     <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="22" t="s">
+      <c r="C20" s="23"/>
+      <c r="D20" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="41" t="s">
+      <c r="E20" s="27"/>
+      <c r="F20" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="41"/>
+      <c r="G20" s="40"/>
     </row>
     <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="42">
-        <v>0</v>
-      </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="42">
+      <c r="A21" s="30"/>
+      <c r="B21" s="24">
+        <v>0</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="24">
         <v>4</v>
       </c>
-      <c r="E21" s="43"/>
-      <c r="F21" s="37">
-        <v>5</v>
-      </c>
-      <c r="G21" s="37"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="41">
+        <v>5</v>
+      </c>
+      <c r="G21" s="41"/>
     </row>
     <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="22" t="s">
+      <c r="B22" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="41" t="s">
+      <c r="E22" s="27"/>
+      <c r="F22" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="41"/>
+      <c r="G22" s="40"/>
     </row>
     <row r="23" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44"/>
-      <c r="B23" s="27">
-        <v>0</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="27">
+      <c r="A23" s="55"/>
+      <c r="B23" s="28">
+        <v>0</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="28">
         <v>2</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="45">
+      <c r="E23" s="29"/>
+      <c r="F23" s="36">
         <v>3</v>
       </c>
-      <c r="G23" s="45"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="22" t="s">
+      <c r="B24" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="23"/>
+      <c r="D24" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="41" t="s">
+      <c r="E24" s="27"/>
+      <c r="F24" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="41"/>
+      <c r="G24" s="40"/>
     </row>
     <row r="25" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="56"/>
-      <c r="B25" s="27">
-        <v>0</v>
-      </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="27">
+      <c r="A25" s="57"/>
+      <c r="B25" s="28">
+        <v>0</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="28">
         <v>2</v>
       </c>
-      <c r="E25" s="28"/>
-      <c r="F25" s="45">
+      <c r="E25" s="29"/>
+      <c r="F25" s="36">
         <v>3</v>
       </c>
-      <c r="G25" s="45"/>
+      <c r="G25" s="36"/>
     </row>
     <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="51"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="52" t="s">
+      <c r="F26" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="52"/>
+      <c r="G26" s="56"/>
     </row>
     <row r="27" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="38"/>
-      <c r="B27" s="42">
-        <v>0</v>
-      </c>
-      <c r="C27" s="43"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="24">
+        <v>0</v>
+      </c>
+      <c r="C27" s="25"/>
       <c r="D27" s="2">
         <v>6</v>
       </c>
       <c r="E27" s="2">
         <v>8</v>
       </c>
-      <c r="F27" s="37">
+      <c r="F27" s="41">
         <v>10</v>
       </c>
-      <c r="G27" s="37"/>
+      <c r="G27" s="41"/>
     </row>
     <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="53" t="s">
+      <c r="A28" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="22" t="s">
+      <c r="B28" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="53"/>
+      <c r="D28" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="55" t="s">
+      <c r="E28" s="27"/>
+      <c r="F28" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="55"/>
+      <c r="G28" s="54"/>
     </row>
     <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="42">
-        <v>0</v>
-      </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="42">
-        <v>5</v>
-      </c>
-      <c r="E29" s="43"/>
-      <c r="F29" s="37">
+      <c r="A29" s="34"/>
+      <c r="B29" s="24">
+        <v>0</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="24">
+        <v>5</v>
+      </c>
+      <c r="E29" s="25"/>
+      <c r="F29" s="41">
         <v>7</v>
       </c>
-      <c r="G29" s="37"/>
+      <c r="G29" s="41"/>
     </row>
     <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="22" t="s">
+      <c r="B30" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="41" t="s">
+      <c r="E30" s="27"/>
+      <c r="F30" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G30" s="41"/>
+      <c r="G30" s="40"/>
     </row>
     <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
-      <c r="B31" s="42">
-        <v>0</v>
-      </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="42">
+      <c r="A31" s="34"/>
+      <c r="B31" s="24">
+        <v>0</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="24">
         <v>3</v>
       </c>
-      <c r="E31" s="43"/>
-      <c r="F31" s="37">
-        <v>5</v>
-      </c>
-      <c r="G31" s="37"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="41">
+        <v>5</v>
+      </c>
+      <c r="G31" s="41"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="54" t="s">
+      <c r="A32" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="22" t="s">
+      <c r="B32" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="23"/>
+      <c r="D32" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="41" t="s">
+      <c r="E32" s="27"/>
+      <c r="F32" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="41"/>
+      <c r="G32" s="40"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
-      <c r="B33" s="35">
-        <v>0</v>
-      </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="35">
+      <c r="A33" s="34"/>
+      <c r="B33" s="49">
+        <v>0</v>
+      </c>
+      <c r="C33" s="50"/>
+      <c r="D33" s="49">
         <v>3</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="49">
-        <v>5</v>
-      </c>
-      <c r="G33" s="49"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="43">
+        <v>5</v>
+      </c>
+      <c r="G33" s="43"/>
     </row>
     <row r="34" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="22" t="s">
+      <c r="B34" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="23"/>
-      <c r="F34" s="26" t="s">
+      <c r="E34" s="27"/>
+      <c r="F34" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G34" s="26"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="57"/>
-      <c r="B35" s="42">
-        <v>0</v>
-      </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="42">
+      <c r="A35" s="35"/>
+      <c r="B35" s="24">
+        <v>0</v>
+      </c>
+      <c r="C35" s="25"/>
+      <c r="D35" s="24">
         <v>2</v>
       </c>
-      <c r="E35" s="43"/>
-      <c r="F35" s="45">
+      <c r="E35" s="25"/>
+      <c r="F35" s="36">
         <v>3</v>
       </c>
-      <c r="G35" s="45"/>
+      <c r="G35" s="36"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="54" t="s">
+      <c r="A36" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="22" t="s">
+      <c r="B36" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="27"/>
+      <c r="D36" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="26" t="s">
+      <c r="E36" s="27"/>
+      <c r="F36" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="26"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="57"/>
-      <c r="B37" s="27">
-        <v>0</v>
-      </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="27">
+      <c r="A37" s="35"/>
+      <c r="B37" s="28">
+        <v>0</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="28">
         <v>2</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="45">
+      <c r="E37" s="29"/>
+      <c r="F37" s="36">
         <v>3</v>
       </c>
-      <c r="G37" s="45"/>
+      <c r="G37" s="36"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="22" t="s">
+      <c r="B38" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="47"/>
+      <c r="D38" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="23"/>
+      <c r="E38" s="27"/>
       <c r="F38" s="48" t="s">
         <v>6</v>
       </c>
       <c r="G38" s="48"/>
     </row>
     <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
-      <c r="B39" s="35">
-        <v>0</v>
-      </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="35">
+      <c r="A39" s="30"/>
+      <c r="B39" s="49">
+        <v>0</v>
+      </c>
+      <c r="C39" s="50"/>
+      <c r="D39" s="49">
         <v>2</v>
       </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="49">
+      <c r="E39" s="50"/>
+      <c r="F39" s="43">
         <v>4</v>
       </c>
-      <c r="G39" s="49"/>
+      <c r="G39" s="43"/>
     </row>
     <row r="40" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="58" t="s">
+      <c r="B40" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="58" t="s">
+      <c r="C40" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="58" t="s">
+      <c r="D40" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E40" s="58" t="s">
+      <c r="E40" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="58" t="s">
+      <c r="F40" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="G40" s="58" t="s">
+      <c r="G40" s="37" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="49"/>
-      <c r="B41" s="59"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
     </row>
     <row r="42" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="49"/>
-      <c r="B42" s="60"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="60"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
     </row>
     <row r="43" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="49"/>
+      <c r="A43" s="43"/>
       <c r="B43" s="2">
         <v>0</v>
       </c>
@@ -1922,48 +1922,48 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="62" t="s">
+      <c r="A44" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B44" s="58" t="s">
+      <c r="B44" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="58" t="s">
+      <c r="C44" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="58" t="s">
+      <c r="D44" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="58" t="s">
+      <c r="E44" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F44" s="58" t="s">
+      <c r="F44" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="G44" s="58" t="s">
+      <c r="G44" s="37" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="59"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="37"/>
-      <c r="B46" s="60"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
-      <c r="G46" s="60"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
     </row>
     <row r="47" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="37"/>
+      <c r="A47" s="41"/>
       <c r="B47" s="2">
         <v>0</v>
       </c>
@@ -1984,48 +1984,48 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30" t="s">
+      <c r="A48" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="58" t="s">
+      <c r="C48" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="58" t="s">
+      <c r="D48" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E48" s="58" t="s">
+      <c r="E48" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F48" s="58" t="s">
+      <c r="F48" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="G48" s="58" t="s">
+      <c r="G48" s="37" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="49"/>
-      <c r="B49" s="59"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="59"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="59"/>
+      <c r="A49" s="43"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="38"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="49"/>
-      <c r="B50" s="60"/>
-      <c r="C50" s="60"/>
-      <c r="D50" s="60"/>
-      <c r="E50" s="60"/>
-      <c r="F50" s="60"/>
-      <c r="G50" s="60"/>
+      <c r="A50" s="43"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
     </row>
     <row r="51" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="49"/>
+      <c r="A51" s="43"/>
       <c r="B51" s="2">
         <v>0</v>
       </c>
@@ -2046,118 +2046,235 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="38" t="s">
+      <c r="A52" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B52" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="40"/>
-      <c r="D52" s="39" t="s">
+      <c r="B52" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="23"/>
+      <c r="D52" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E52" s="40"/>
-      <c r="F52" s="41" t="s">
+      <c r="E52" s="23"/>
+      <c r="F52" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="41"/>
+      <c r="G52" s="40"/>
     </row>
     <row r="53" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="38"/>
-      <c r="B53" s="42">
-        <v>0</v>
-      </c>
-      <c r="C53" s="43"/>
-      <c r="D53" s="42">
+      <c r="A53" s="30"/>
+      <c r="B53" s="24">
+        <v>0</v>
+      </c>
+      <c r="C53" s="25"/>
+      <c r="D53" s="24">
         <v>1</v>
       </c>
-      <c r="E53" s="43"/>
-      <c r="F53" s="37">
+      <c r="E53" s="25"/>
+      <c r="F53" s="41">
         <v>3</v>
       </c>
-      <c r="G53" s="37"/>
+      <c r="G53" s="41"/>
     </row>
     <row r="54" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="38" t="s">
+      <c r="A54" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B54" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="23"/>
-      <c r="D54" s="22" t="s">
+      <c r="B54" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="27"/>
+      <c r="D54" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E54" s="23"/>
-      <c r="F54" s="26" t="s">
+      <c r="E54" s="27"/>
+      <c r="F54" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G54" s="26"/>
+      <c r="G54" s="32"/>
     </row>
     <row r="55" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="61"/>
-      <c r="B55" s="27">
-        <v>0</v>
-      </c>
-      <c r="C55" s="28"/>
-      <c r="D55" s="27">
+      <c r="A55" s="31"/>
+      <c r="B55" s="28">
+        <v>0</v>
+      </c>
+      <c r="C55" s="29"/>
+      <c r="D55" s="28">
         <v>1</v>
       </c>
-      <c r="E55" s="28"/>
-      <c r="F55" s="29">
+      <c r="E55" s="29"/>
+      <c r="F55" s="33">
         <v>3</v>
       </c>
-      <c r="G55" s="29"/>
+      <c r="G55" s="33"/>
     </row>
     <row r="56" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C56" s="23"/>
-      <c r="D56" s="24" t="s">
+      <c r="C56" s="27"/>
+      <c r="D56" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="E56" s="47"/>
+      <c r="F56" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="E56" s="25"/>
-      <c r="F56" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="G56" s="26"/>
+      <c r="G56" s="32"/>
     </row>
     <row r="57" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B57" s="27" t="s">
+      <c r="B57" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="28"/>
-      <c r="D57" s="27" t="s">
+      <c r="C57" s="29"/>
+      <c r="D57" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E57" s="28"/>
-      <c r="F57" s="29" t="s">
+      <c r="E57" s="29"/>
+      <c r="F57" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G57" s="29"/>
+      <c r="G57" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="167">
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="F4:G5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="D17:E18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="F54:G54"/>
@@ -2182,136 +2299,19 @@
     <mergeCell ref="F48:F50"/>
     <mergeCell ref="G40:G42"/>
     <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="D17:E18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:E5"/>
-    <mergeCell ref="F4:G5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2353,7 +2353,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="45" t="s">
         <v>52</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2370,7 +2370,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="13">
         <v>0</v>
       </c>
@@ -2385,7 +2385,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="33" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="45" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -2402,7 +2402,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="13">
         <v>0</v>
       </c>
@@ -2417,7 +2417,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="45" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -2434,7 +2434,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="13">
         <v>0</v>
       </c>
@@ -2449,7 +2449,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="45" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -2466,7 +2466,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="13">
         <v>0</v>
       </c>
@@ -2481,7 +2481,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="45" t="s">
         <v>64</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -2498,7 +2498,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="13">
         <v>0</v>
       </c>
@@ -2513,7 +2513,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="45" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -2530,7 +2530,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="16">
         <v>0</v>
       </c>
@@ -2595,8 +2595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4767C49-F7BD-4CA8-80E6-FC837B1E66A5}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>84</v>

</xml_diff>